<commit_message>
Feat: Normalização da tabela de musicas favoritas e criação da mesma
</commit_message>
<xml_diff>
--- a/SpotifyClone-modelagem.xlsx
+++ b/SpotifyClone-modelagem.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t xml:space="preserve">usuarios</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t xml:space="preserve">"2015-12-13 08:30:22"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cancoes_favoritas</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -397,19 +400,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF860D"/>
       <name val="Calibri"/>
@@ -417,7 +407,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,7 +423,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFA6A6"/>
-        <bgColor rgb="FFFF8080"/>
+        <bgColor rgb="FFE0C2CD"/>
       </patternFill>
     </fill>
     <fill>
@@ -451,7 +441,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF6D"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -464,6 +454,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8E86AE"/>
         <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0C2CD"/>
+        <bgColor rgb="FFF7D1D5"/>
       </patternFill>
     </fill>
   </fills>
@@ -557,7 +553,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -694,7 +690,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -730,15 +726,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,11 +738,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,7 +778,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -799,22 +787,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,15 +806,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,7 +818,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -887,12 +863,12 @@
       <rgbColor rgb="FF8E86AE"/>
       <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFF7D1D5"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF2A6099"/>
-      <rgbColor rgb="FFF7D1D5"/>
+      <rgbColor rgb="FFE0C2CD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -937,14 +913,14 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D74" activeCellId="0" sqref="D74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B106" activeCellId="0" sqref="A93:B106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="28.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="28.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.3"/>
@@ -1384,7 +1360,7 @@
       <c r="A26" s="42" t="n">
         <v>4</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="17" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="0"/>
@@ -1396,7 +1372,7 @@
       <c r="A27" s="42" t="n">
         <v>5</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="0"/>
@@ -1405,10 +1381,10 @@
       <c r="I27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="44" t="n">
+      <c r="A28" s="43" t="n">
         <v>6</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="0"/>
@@ -1425,8 +1401,8 @@
       <c r="I29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47" t="s">
+      <c r="A30" s="44"/>
+      <c r="B30" s="45" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="32"/>
@@ -1435,10 +1411,10 @@
       <c r="I30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="32"/>
@@ -1645,7 +1621,7 @@
       <c r="A45" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="B45" s="50" t="n">
+      <c r="B45" s="48" t="n">
         <v>2</v>
       </c>
       <c r="C45" s="0"/>
@@ -1664,12 +1640,12 @@
       <c r="I46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="51"/>
-      <c r="B47" s="52" t="s">
+      <c r="A47" s="49"/>
+      <c r="B47" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="53"/>
-      <c r="D47" s="54"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="52"/>
       <c r="E47" s="0"/>
       <c r="H47" s="31"/>
       <c r="I47" s="32"/>
@@ -1684,7 +1660,7 @@
       <c r="C48" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="55" t="s">
+      <c r="D48" s="53" t="s">
         <v>36</v>
       </c>
       <c r="E48" s="0"/>
@@ -1846,12 +1822,12 @@
       <c r="I58" s="32"/>
     </row>
     <row r="59" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="56"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="58" t="s">
+      <c r="A59" s="54"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="59"/>
+      <c r="D59" s="57"/>
       <c r="E59" s="0"/>
       <c r="H59" s="31"/>
       <c r="I59" s="32"/>
@@ -1866,7 +1842,7 @@
       <c r="C60" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D60" s="60" t="s">
+      <c r="D60" s="58" t="s">
         <v>46</v>
       </c>
       <c r="E60" s="0"/>
@@ -1877,10 +1853,10 @@
       <c r="A61" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="B61" s="61" t="s">
+      <c r="B61" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C61" s="62" t="n">
+      <c r="C61" s="14" t="n">
         <v>279</v>
       </c>
       <c r="D61" s="37" t="n">
@@ -1894,10 +1870,10 @@
       <c r="A62" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="B62" s="63" t="s">
+      <c r="B62" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="61" t="n">
+      <c r="C62" s="15" t="n">
         <v>369</v>
       </c>
       <c r="D62" s="37" t="n">
@@ -1911,10 +1887,10 @@
       <c r="A63" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="B63" s="63" t="s">
+      <c r="B63" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="61" t="n">
+      <c r="C63" s="15" t="n">
         <v>116</v>
       </c>
       <c r="D63" s="37" t="n">
@@ -1928,7 +1904,7 @@
       <c r="A64" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="B64" s="63" t="s">
+      <c r="B64" s="23" t="s">
         <v>71</v>
       </c>
       <c r="C64" s="15" t="n">
@@ -1945,7 +1921,7 @@
       <c r="A65" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="B65" s="63" t="s">
+      <c r="B65" s="23" t="s">
         <v>72</v>
       </c>
       <c r="C65" s="15" t="n">
@@ -1962,7 +1938,7 @@
       <c r="A66" s="22" t="n">
         <v>6</v>
       </c>
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="23" t="s">
         <v>73</v>
       </c>
       <c r="C66" s="15" t="n">
@@ -1979,7 +1955,7 @@
       <c r="A67" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="B67" s="63" t="s">
+      <c r="B67" s="23" t="s">
         <v>74</v>
       </c>
       <c r="C67" s="15" t="n">
@@ -1996,7 +1972,7 @@
       <c r="A68" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B68" s="63" t="s">
+      <c r="B68" s="23" t="s">
         <v>75</v>
       </c>
       <c r="C68" s="15" t="n">
@@ -2013,7 +1989,7 @@
       <c r="A69" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="B69" s="63" t="s">
+      <c r="B69" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C69" s="15" t="n">
@@ -2030,7 +2006,7 @@
       <c r="A70" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="B70" s="64" t="s">
+      <c r="B70" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C70" s="28" t="n">
@@ -2047,33 +2023,33 @@
       <c r="A71" s="0"/>
       <c r="B71" s="0"/>
       <c r="C71" s="0"/>
-      <c r="D71" s="65"/>
+      <c r="D71" s="59"/>
       <c r="E71" s="32"/>
       <c r="H71" s="31"/>
       <c r="I71" s="32"/>
     </row>
     <row r="72" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="66"/>
-      <c r="B72" s="67" t="s">
+      <c r="A72" s="60"/>
+      <c r="B72" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="C72" s="68"/>
-      <c r="D72" s="65"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="59"/>
       <c r="E72" s="32"/>
       <c r="H72" s="31"/>
       <c r="I72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="69" t="s">
+      <c r="A73" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="70" t="s">
+      <c r="B73" s="64" t="s">
         <v>65</v>
       </c>
       <c r="C73" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D73" s="65"/>
+      <c r="D73" s="59"/>
       <c r="E73" s="32"/>
       <c r="H73" s="31"/>
       <c r="I73" s="32"/>
@@ -2085,10 +2061,10 @@
       <c r="B74" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="C74" s="71" t="s">
+      <c r="C74" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D74" s="65"/>
+      <c r="D74" s="59"/>
       <c r="E74" s="32"/>
       <c r="H74" s="31"/>
       <c r="I74" s="32"/>
@@ -2100,10 +2076,10 @@
       <c r="B75" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C75" s="71" t="s">
+      <c r="C75" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D75" s="65"/>
+      <c r="D75" s="59"/>
       <c r="E75" s="32"/>
       <c r="H75" s="31"/>
       <c r="I75" s="32"/>
@@ -2115,7 +2091,7 @@
       <c r="B76" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="C76" s="71" t="s">
+      <c r="C76" s="37" t="s">
         <v>82</v>
       </c>
       <c r="E76" s="32"/>
@@ -2129,10 +2105,10 @@
       <c r="B77" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="C77" s="71" t="s">
+      <c r="C77" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="D77" s="65"/>
+      <c r="D77" s="59"/>
       <c r="E77" s="32"/>
       <c r="H77" s="31"/>
       <c r="I77" s="32"/>
@@ -2144,10 +2120,10 @@
       <c r="B78" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="C78" s="71" t="s">
+      <c r="C78" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="D78" s="65"/>
+      <c r="D78" s="59"/>
       <c r="E78" s="32"/>
       <c r="H78" s="31"/>
       <c r="I78" s="32"/>
@@ -2159,7 +2135,7 @@
       <c r="B79" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="C79" s="71" t="s">
+      <c r="C79" s="37" t="s">
         <v>85</v>
       </c>
       <c r="E79" s="32"/>
@@ -2173,7 +2149,7 @@
       <c r="B80" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C80" s="71" t="s">
+      <c r="C80" s="37" t="s">
         <v>86</v>
       </c>
       <c r="E80" s="32"/>
@@ -2187,7 +2163,7 @@
       <c r="B81" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="C81" s="71" t="s">
+      <c r="C81" s="37" t="s">
         <v>87</v>
       </c>
       <c r="E81" s="32"/>
@@ -2201,7 +2177,7 @@
       <c r="B82" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="C82" s="71" t="s">
+      <c r="C82" s="37" t="s">
         <v>88</v>
       </c>
       <c r="E82" s="32"/>
@@ -2229,7 +2205,7 @@
       <c r="B84" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="C84" s="71" t="s">
+      <c r="C84" s="37" t="s">
         <v>90</v>
       </c>
       <c r="E84" s="32"/>
@@ -2237,13 +2213,13 @@
       <c r="I84" s="32"/>
     </row>
     <row r="85" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="72" t="n">
+      <c r="A85" s="65" t="n">
         <v>6</v>
       </c>
       <c r="B85" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="C85" s="71" t="s">
+      <c r="C85" s="37" t="s">
         <v>91</v>
       </c>
       <c r="E85" s="32"/>
@@ -2257,7 +2233,7 @@
       <c r="B86" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="C86" s="71" t="s">
+      <c r="C86" s="37" t="s">
         <v>92</v>
       </c>
       <c r="E86" s="32"/>
@@ -2271,7 +2247,7 @@
       <c r="B87" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="C87" s="71" t="s">
+      <c r="C87" s="37" t="s">
         <v>93</v>
       </c>
       <c r="E87" s="32"/>
@@ -2285,7 +2261,7 @@
       <c r="B88" s="23" t="n">
         <v>9</v>
       </c>
-      <c r="C88" s="71" t="s">
+      <c r="C88" s="37" t="s">
         <v>94</v>
       </c>
       <c r="E88" s="32"/>
@@ -2299,7 +2275,7 @@
       <c r="B89" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="C89" s="73" t="s">
+      <c r="C89" s="38" t="s">
         <v>95</v>
       </c>
       <c r="E89" s="32"/>
@@ -2323,192 +2299,244 @@
       <c r="I91" s="32"/>
     </row>
     <row r="92" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0"/>
-      <c r="B92" s="0"/>
+      <c r="A92" s="66"/>
+      <c r="B92" s="67" t="s">
+        <v>96</v>
+      </c>
       <c r="C92" s="0"/>
       <c r="E92" s="32"/>
       <c r="H92" s="31"/>
       <c r="I92" s="32"/>
     </row>
     <row r="93" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0"/>
-      <c r="B93" s="0"/>
-      <c r="C93" s="0"/>
+      <c r="A93" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C93" s="22"/>
+      <c r="D93" s="15"/>
       <c r="E93" s="32"/>
       <c r="H93" s="31"/>
       <c r="I93" s="32"/>
     </row>
     <row r="94" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0"/>
-      <c r="B94" s="0"/>
+      <c r="A94" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="B94" s="68" t="n">
+        <v>3</v>
+      </c>
       <c r="C94" s="0"/>
       <c r="E94" s="32"/>
       <c r="H94" s="31"/>
       <c r="I94" s="32"/>
     </row>
     <row r="95" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0"/>
-      <c r="B95" s="0"/>
+      <c r="A95" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="B95" s="68" t="n">
+        <v>6</v>
+      </c>
       <c r="C95" s="0"/>
       <c r="E95" s="32"/>
       <c r="H95" s="31"/>
       <c r="I95" s="32"/>
     </row>
     <row r="96" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0"/>
-      <c r="B96" s="0"/>
+      <c r="A96" s="42" t="n">
+        <v>1</v>
+      </c>
+      <c r="B96" s="68" t="n">
+        <v>10</v>
+      </c>
       <c r="C96" s="0"/>
       <c r="E96" s="32"/>
       <c r="H96" s="31"/>
       <c r="I96" s="32"/>
     </row>
     <row r="97" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0"/>
-      <c r="B97" s="0"/>
+      <c r="A97" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="B97" s="68" t="n">
+        <v>4</v>
+      </c>
       <c r="C97" s="0"/>
       <c r="E97" s="32"/>
       <c r="H97" s="31"/>
       <c r="I97" s="32"/>
     </row>
     <row r="98" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0"/>
-      <c r="B98" s="0"/>
+      <c r="A98" s="42" t="n">
+        <v>3</v>
+      </c>
+      <c r="B98" s="68" t="n">
+        <v>1</v>
+      </c>
       <c r="C98" s="0"/>
       <c r="E98" s="32"/>
       <c r="H98" s="31"/>
       <c r="I98" s="32"/>
     </row>
     <row r="99" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0"/>
-      <c r="B99" s="0"/>
+      <c r="A99" s="42" t="n">
+        <v>3</v>
+      </c>
+      <c r="B99" s="68" t="n">
+        <v>3</v>
+      </c>
       <c r="C99" s="0"/>
       <c r="E99" s="32"/>
       <c r="H99" s="31"/>
       <c r="I99" s="32"/>
     </row>
     <row r="100" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0"/>
-      <c r="B100" s="0"/>
+      <c r="A100" s="42" t="n">
+        <v>4</v>
+      </c>
+      <c r="B100" s="68" t="n">
+        <v>7</v>
+      </c>
       <c r="C100" s="0"/>
       <c r="E100" s="32"/>
       <c r="H100" s="31"/>
       <c r="I100" s="32"/>
     </row>
     <row r="101" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0"/>
-      <c r="B101" s="0"/>
+      <c r="A101" s="42" t="n">
+        <v>4</v>
+      </c>
+      <c r="B101" s="68" t="n">
+        <v>4</v>
+      </c>
       <c r="C101" s="0"/>
       <c r="E101" s="32"/>
       <c r="H101" s="31"/>
       <c r="I101" s="32"/>
     </row>
     <row r="102" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0"/>
-      <c r="B102" s="0"/>
+      <c r="A102" s="42" t="n">
+        <v>5</v>
+      </c>
+      <c r="B102" s="68" t="n">
+        <v>10</v>
+      </c>
       <c r="C102" s="0"/>
       <c r="E102" s="32"/>
       <c r="H102" s="31"/>
       <c r="I102" s="32"/>
     </row>
     <row r="103" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0"/>
-      <c r="B103" s="0"/>
+      <c r="A103" s="42" t="n">
+        <v>5</v>
+      </c>
+      <c r="B103" s="68" t="n">
+        <v>2</v>
+      </c>
       <c r="C103" s="0"/>
       <c r="E103" s="32"/>
       <c r="H103" s="31"/>
       <c r="I103" s="32"/>
     </row>
     <row r="104" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0"/>
-      <c r="B104" s="0"/>
+      <c r="A104" s="42" t="n">
+        <v>8</v>
+      </c>
+      <c r="B104" s="68" t="n">
+        <v>4</v>
+      </c>
       <c r="C104" s="0"/>
       <c r="E104" s="32"/>
       <c r="H104" s="31"/>
       <c r="I104" s="32"/>
     </row>
     <row r="105" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="21"/>
-      <c r="B105" s="65"/>
-      <c r="C105" s="0"/>
+      <c r="A105" s="42" t="n">
+        <v>9</v>
+      </c>
+      <c r="B105" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C105" s="32"/>
       <c r="E105" s="32"/>
       <c r="H105" s="31"/>
       <c r="I105" s="32"/>
     </row>
     <row r="106" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="21"/>
-      <c r="B106" s="65"/>
-      <c r="C106" s="0"/>
+      <c r="A106" s="43" t="n">
+        <v>10</v>
+      </c>
+      <c r="B106" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C106" s="32"/>
       <c r="E106" s="32"/>
       <c r="H106" s="31"/>
       <c r="I106" s="32"/>
     </row>
     <row r="107" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="21"/>
-      <c r="B107" s="74"/>
+      <c r="B107" s="69"/>
       <c r="C107" s="0"/>
       <c r="E107" s="32"/>
       <c r="H107" s="31"/>
       <c r="I107" s="32"/>
     </row>
     <row r="108" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="21"/>
-      <c r="B108" s="22"/>
-      <c r="C108" s="0"/>
+      <c r="A108" s="59"/>
+      <c r="B108" s="59"/>
+      <c r="C108" s="32"/>
       <c r="E108" s="32"/>
       <c r="H108" s="31"/>
       <c r="I108" s="32"/>
     </row>
     <row r="109" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="21"/>
-      <c r="B109" s="22"/>
-      <c r="C109" s="0"/>
+      <c r="A109" s="32"/>
+      <c r="C109" s="32"/>
       <c r="E109" s="32"/>
       <c r="H109" s="31"/>
       <c r="I109" s="32"/>
     </row>
     <row r="110" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="2"/>
-      <c r="B110" s="22"/>
-      <c r="C110" s="0"/>
+      <c r="A110" s="32"/>
+      <c r="C110" s="32"/>
       <c r="E110" s="32"/>
       <c r="H110" s="31"/>
       <c r="I110" s="32"/>
     </row>
     <row r="111" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="32"/>
-      <c r="B111" s="22"/>
-      <c r="C111" s="0"/>
+      <c r="C111" s="32"/>
       <c r="E111" s="32"/>
       <c r="H111" s="31"/>
       <c r="I111" s="32"/>
     </row>
     <row r="112" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="32"/>
-      <c r="B112" s="22"/>
-      <c r="C112" s="0"/>
+      <c r="C112" s="32"/>
       <c r="E112" s="32"/>
       <c r="H112" s="31"/>
       <c r="I112" s="32"/>
     </row>
     <row r="113" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="32"/>
-      <c r="B113" s="22"/>
-      <c r="C113" s="0"/>
+      <c r="C113" s="32"/>
       <c r="E113" s="32"/>
       <c r="H113" s="31"/>
       <c r="I113" s="32"/>
     </row>
     <row r="114" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="32"/>
-      <c r="B114" s="22"/>
-      <c r="C114" s="0"/>
+      <c r="C114" s="32"/>
       <c r="E114" s="32"/>
       <c r="H114" s="31"/>
       <c r="I114" s="32"/>
     </row>
     <row r="115" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="32"/>
-      <c r="B115" s="22"/>
       <c r="C115" s="32"/>
       <c r="E115" s="32"/>
       <c r="H115" s="31"/>
@@ -2516,7 +2544,6 @@
     </row>
     <row r="116" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="32"/>
-      <c r="B116" s="22"/>
       <c r="C116" s="32"/>
       <c r="E116" s="32"/>
       <c r="H116" s="31"/>
@@ -2524,86 +2551,84 @@
     </row>
     <row r="117" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="32"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="0"/>
+      <c r="C117" s="32"/>
       <c r="E117" s="32"/>
       <c r="H117" s="31"/>
       <c r="I117" s="32"/>
     </row>
     <row r="118" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="32"/>
-      <c r="B118" s="0"/>
-      <c r="C118" s="61"/>
+      <c r="C118" s="32"/>
       <c r="E118" s="32"/>
       <c r="H118" s="31"/>
       <c r="I118" s="32"/>
     </row>
     <row r="119" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="32"/>
-      <c r="C119" s="63"/>
+      <c r="C119" s="32"/>
       <c r="E119" s="32"/>
       <c r="H119" s="31"/>
       <c r="I119" s="32"/>
     </row>
     <row r="120" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="32"/>
-      <c r="C120" s="63"/>
+      <c r="C120" s="32"/>
       <c r="E120" s="32"/>
       <c r="H120" s="31"/>
       <c r="I120" s="32"/>
     </row>
     <row r="121" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="32"/>
-      <c r="C121" s="63"/>
+      <c r="C121" s="32"/>
       <c r="E121" s="32"/>
       <c r="H121" s="31"/>
       <c r="I121" s="32"/>
     </row>
     <row r="122" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="32"/>
-      <c r="C122" s="63"/>
+      <c r="C122" s="32"/>
       <c r="E122" s="32"/>
       <c r="H122" s="31"/>
       <c r="I122" s="32"/>
     </row>
     <row r="123" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="32"/>
-      <c r="C123" s="63"/>
+      <c r="C123" s="32"/>
       <c r="E123" s="32"/>
       <c r="H123" s="31"/>
       <c r="I123" s="32"/>
     </row>
     <row r="124" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="32"/>
-      <c r="C124" s="63"/>
+      <c r="C124" s="32"/>
       <c r="E124" s="32"/>
       <c r="H124" s="31"/>
       <c r="I124" s="32"/>
     </row>
     <row r="125" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="32"/>
-      <c r="C125" s="63"/>
+      <c r="C125" s="32"/>
       <c r="E125" s="32"/>
       <c r="H125" s="31"/>
       <c r="I125" s="32"/>
     </row>
     <row r="126" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="32"/>
-      <c r="C126" s="63"/>
+      <c r="C126" s="32"/>
       <c r="E126" s="32"/>
       <c r="H126" s="31"/>
       <c r="I126" s="32"/>
     </row>
     <row r="127" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="32"/>
-      <c r="C127" s="64"/>
+      <c r="C127" s="32"/>
       <c r="E127" s="32"/>
       <c r="H127" s="31"/>
       <c r="I127" s="32"/>
     </row>
     <row r="128" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="32"/>
-      <c r="C128" s="0"/>
+      <c r="C128" s="32"/>
       <c r="E128" s="32"/>
       <c r="H128" s="31"/>
       <c r="I128" s="32"/>
@@ -8538,166 +8563,126 @@
       <c r="I975" s="32"/>
     </row>
     <row r="976" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A976" s="32"/>
-      <c r="C976" s="32"/>
       <c r="E976" s="32"/>
       <c r="H976" s="31"/>
       <c r="I976" s="32"/>
     </row>
     <row r="977" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A977" s="32"/>
-      <c r="C977" s="32"/>
       <c r="E977" s="32"/>
       <c r="H977" s="31"/>
       <c r="I977" s="32"/>
     </row>
     <row r="978" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A978" s="32"/>
-      <c r="C978" s="32"/>
       <c r="E978" s="32"/>
       <c r="H978" s="31"/>
       <c r="I978" s="32"/>
     </row>
     <row r="979" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A979" s="32"/>
-      <c r="C979" s="32"/>
       <c r="E979" s="32"/>
       <c r="H979" s="31"/>
       <c r="I979" s="32"/>
     </row>
     <row r="980" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A980" s="32"/>
-      <c r="C980" s="32"/>
       <c r="E980" s="32"/>
       <c r="H980" s="31"/>
       <c r="I980" s="32"/>
     </row>
     <row r="981" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A981" s="32"/>
-      <c r="C981" s="32"/>
       <c r="E981" s="32"/>
       <c r="H981" s="31"/>
       <c r="I981" s="32"/>
     </row>
     <row r="982" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A982" s="32"/>
-      <c r="C982" s="32"/>
       <c r="E982" s="32"/>
       <c r="H982" s="31"/>
       <c r="I982" s="32"/>
     </row>
     <row r="983" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A983" s="32"/>
-      <c r="C983" s="32"/>
       <c r="E983" s="32"/>
       <c r="H983" s="31"/>
       <c r="I983" s="32"/>
     </row>
     <row r="984" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A984" s="32"/>
-      <c r="C984" s="32"/>
       <c r="E984" s="32"/>
       <c r="H984" s="31"/>
       <c r="I984" s="32"/>
     </row>
     <row r="985" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A985" s="32"/>
-      <c r="C985" s="32"/>
       <c r="E985" s="32"/>
       <c r="H985" s="31"/>
       <c r="I985" s="32"/>
     </row>
     <row r="986" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A986" s="32"/>
-      <c r="C986" s="32"/>
       <c r="E986" s="32"/>
       <c r="H986" s="31"/>
       <c r="I986" s="32"/>
     </row>
     <row r="987" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A987" s="32"/>
-      <c r="C987" s="32"/>
       <c r="E987" s="32"/>
       <c r="H987" s="31"/>
       <c r="I987" s="32"/>
     </row>
     <row r="988" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A988" s="32"/>
-      <c r="C988" s="32"/>
       <c r="E988" s="32"/>
       <c r="H988" s="31"/>
       <c r="I988" s="32"/>
     </row>
     <row r="989" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A989" s="32"/>
-      <c r="C989" s="32"/>
       <c r="E989" s="32"/>
       <c r="H989" s="31"/>
       <c r="I989" s="32"/>
     </row>
     <row r="990" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A990" s="32"/>
-      <c r="C990" s="32"/>
       <c r="E990" s="32"/>
       <c r="H990" s="31"/>
       <c r="I990" s="32"/>
     </row>
     <row r="991" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C991" s="32"/>
       <c r="E991" s="32"/>
       <c r="H991" s="31"/>
       <c r="I991" s="32"/>
     </row>
     <row r="992" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C992" s="32"/>
       <c r="E992" s="32"/>
       <c r="H992" s="31"/>
       <c r="I992" s="32"/>
     </row>
     <row r="993" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C993" s="32"/>
       <c r="E993" s="32"/>
       <c r="H993" s="31"/>
       <c r="I993" s="32"/>
     </row>
     <row r="994" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C994" s="32"/>
       <c r="E994" s="32"/>
       <c r="H994" s="31"/>
       <c r="I994" s="32"/>
     </row>
     <row r="995" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C995" s="32"/>
       <c r="E995" s="32"/>
       <c r="H995" s="31"/>
       <c r="I995" s="32"/>
     </row>
     <row r="996" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C996" s="32"/>
       <c r="E996" s="32"/>
       <c r="H996" s="31"/>
       <c r="I996" s="32"/>
     </row>
     <row r="997" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C997" s="32"/>
       <c r="E997" s="32"/>
       <c r="H997" s="31"/>
       <c r="I997" s="32"/>
     </row>
     <row r="998" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C998" s="32"/>
       <c r="E998" s="32"/>
       <c r="H998" s="31"/>
       <c r="I998" s="32"/>
     </row>
     <row r="999" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C999" s="32"/>
       <c r="E999" s="32"/>
       <c r="H999" s="31"/>
       <c r="I999" s="32"/>
     </row>
     <row r="1000" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1000" s="32"/>
       <c r="E1000" s="32"/>
       <c r="H1000" s="31"/>
       <c r="I1000" s="32"/>

</xml_diff>